<commit_message>
saving excel and word files
</commit_message>
<xml_diff>
--- a/computer_science_and_engineering_first_course_24.1/fundamentals_of_information_technology/pws/excel/pw1/Zadanie1.xlsx
+++ b/computer_science_and_engineering_first_course_24.1/fundamentals_of_information_technology/pws/excel/pw1/Zadanie1.xlsx
@@ -331,8 +331,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$₽-419]_-;\-* #,##0.00\ [$₽-419]_-;_-* &quot;-&quot;??\ [$₽-419]_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -406,15 +406,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -427,15 +427,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -763,7 +763,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1411,16 +1411,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1718,21 +1718,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2898,7 +2898,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,15 +2913,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3221,31 +3221,31 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11">
         <v>48.6</v>
       </c>
     </row>
@@ -3384,7 +3384,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="1">

</xml_diff>